<commit_message>
version completa para importar articulos
</commit_message>
<xml_diff>
--- a/tmp/pedimentos.xlsx
+++ b/tmp/pedimentos.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="20055" windowHeight="8655" tabRatio="504"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="21255" windowHeight="10440"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -16,30 +16,51 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="13">
+  <si>
+    <t>AICM</t>
+  </si>
+  <si>
+    <t>12/19/2013</t>
+  </si>
+  <si>
+    <t>lote-01</t>
+  </si>
+  <si>
+    <t>lote-02</t>
+  </si>
+  <si>
+    <t>lote-03</t>
+  </si>
+  <si>
+    <t>lote-04</t>
+  </si>
+  <si>
+    <t>lote-05</t>
+  </si>
+  <si>
+    <t>lote-06</t>
+  </si>
+  <si>
+    <t>lote-07</t>
+  </si>
+  <si>
+    <t>lote-08</t>
+  </si>
+  <si>
+    <t>lote-09</t>
+  </si>
+  <si>
+    <t>lote-10</t>
+  </si>
   <si>
     <t>MIAMI</t>
-  </si>
-  <si>
-    <t>AICM</t>
-  </si>
-  <si>
-    <t>13 53 3061 3002049</t>
-  </si>
-  <si>
-    <t>13-802240</t>
-  </si>
-  <si>
-    <t>19/12/2013</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode=";;"/>
-  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -49,18 +70,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <sz val="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <i/>
       <sz val="10"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -80,19 +108,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -391,41 +424,189 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" customWidth="1"/>
-    <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+    <col min="1" max="1" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1">
+        <v>134735223004059</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>135330613002049</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>135330613000307</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>0</v>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>134735223002677</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>135330613001327</v>
+      </c>
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>135330613000523</v>
+      </c>
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>134735223000061</v>
+      </c>
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>134735223000062</v>
+      </c>
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>124735222003488</v>
+      </c>
+      <c r="B9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>124735222003487</v>
+      </c>
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
se valida que si estan vacios no haga nada
</commit_message>
<xml_diff>
--- a/tmp/pedimentos.xlsx
+++ b/tmp/pedimentos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="21255" windowHeight="10440"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="9255" windowHeight="8550" tabRatio="504"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -16,51 +16,72 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>AICM</t>
   </si>
   <si>
+    <t>13-802240</t>
+  </si>
+  <si>
+    <t>CANCUN</t>
+  </si>
+  <si>
+    <t>12-03350</t>
+  </si>
+  <si>
+    <t>12-03288</t>
+  </si>
+  <si>
+    <t>13-00085</t>
+  </si>
+  <si>
+    <t>13-03918</t>
+  </si>
+  <si>
+    <t>13-800505</t>
+  </si>
+  <si>
     <t>12/19/2013</t>
   </si>
   <si>
-    <t>lote-01</t>
-  </si>
-  <si>
-    <t>lote-02</t>
-  </si>
-  <si>
-    <t>lote-03</t>
-  </si>
-  <si>
-    <t>lote-04</t>
-  </si>
-  <si>
-    <t>lote-05</t>
-  </si>
-  <si>
-    <t>lote-06</t>
-  </si>
-  <si>
-    <t>lote-07</t>
-  </si>
-  <si>
-    <t>lote-08</t>
-  </si>
-  <si>
-    <t>lote-09</t>
-  </si>
-  <si>
-    <t>lote-10</t>
-  </si>
-  <si>
-    <t>MIAMI</t>
+    <t>12/24/2012</t>
+  </si>
+  <si>
+    <t>02/15/2013</t>
+  </si>
+  <si>
+    <t>12/26/2013</t>
+  </si>
+  <si>
+    <t>03/27/2013</t>
+  </si>
+  <si>
+    <t>124735222003487</t>
+  </si>
+  <si>
+    <t>124735222003488</t>
+  </si>
+  <si>
+    <t>134735223000062</t>
+  </si>
+  <si>
+    <t>134735223004059</t>
+  </si>
+  <si>
+    <t>135330613000523</t>
+  </si>
+  <si>
+    <t>135330613002049</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode=";;"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -70,25 +91,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
     <font>
-      <b/>
-      <i/>
       <sz val="10"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -108,24 +122,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -424,189 +439,126 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" customWidth="1"/>
+    <col min="2" max="2" width="41.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1">
-        <v>134735223004059</v>
+      <c r="A1" s="5" t="s">
+        <v>18</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>135330613002049</v>
+      <c r="A2" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>1</v>
+      <c r="C2" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>135330613000307</v>
+      <c r="A3" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>1</v>
+      <c r="C3" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="D3" t="s">
         <v>4</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>134735223002677</v>
+      <c r="A4" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>1</v>
+      <c r="C4" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>135330613001327</v>
+      <c r="A5" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>1</v>
+      <c r="C5" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="D5" t="s">
         <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>135330613000523</v>
+      <c r="A6" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="B6" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>1</v>
+      <c r="C6" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
       </c>
-      <c r="E6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
-        <v>134735223000061</v>
-      </c>
-      <c r="B7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
-        <v>134735223000062</v>
-      </c>
-      <c r="B8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
-        <v>124735222003488</v>
-      </c>
-      <c r="B9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
-        <v>124735222003487</v>
-      </c>
-      <c r="B10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" t="s">
-        <v>12</v>
+      <c r="E6" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>